<commit_message>
Update PM04 Tidsregistrering for Bille.xlsx
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM04 Tidsregistrering for Bille.xlsx
+++ b/08 Project Management/Tidsregistrering/PM04 Tidsregistrering for Bille.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2C9B44-E2DD-4F9F-8C0D-7D2118E29BBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7509878D-A073-4B1B-B81C-22D6052C729B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9060" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
+    <workbookView xWindow="5208" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="Roller">'Ark2'!$B$3:$B$31</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>Dato</t>
   </si>
@@ -181,6 +184,18 @@
   </si>
   <si>
     <t>Review af XD Phone</t>
+  </si>
+  <si>
+    <t>OC0802</t>
+  </si>
+  <si>
+    <t>KKO use-case møde</t>
+  </si>
+  <si>
+    <t>IndtjeningsBidrag AD møde</t>
+  </si>
+  <si>
+    <t>DOM06 KontantKapacitetsOmkostning</t>
   </si>
 </sst>
 </file>
@@ -737,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EC185-8A27-41F3-967D-179793E73F80}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" thickTop="1" thickBottom="1" x14ac:dyDescent="0.35"/>
@@ -994,57 +1009,107 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="A11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="18">
+        <v>43887</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.44097222222222227</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.5138888888888951E-2</v>
       </c>
       <c r="H11" s="8">
         <f>SUM(G$3:G11)</f>
-        <v>0.28125000000000017</v>
+        <v>0.32638888888888912</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="18">
+        <v>43887</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.46875</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.49652777777777773</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.7777777777777735E-2</v>
       </c>
       <c r="H12" s="8">
         <f>SUM(G$3:G12)</f>
-        <v>0.28125000000000017</v>
+        <v>0.35416666666666685</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="A13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="18">
+        <v>43887</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.54513888888888895</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.4722222222222321E-2</v>
       </c>
       <c r="H13" s="8">
         <f>SUM(G$3:G13)</f>
-        <v>0.28125000000000017</v>
+        <v>0.38888888888888917</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C14" s="2"/>
+      <c r="A14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="18">
+        <v>43887</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.59375</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.208333333333337E-2</v>
       </c>
       <c r="H14" s="8">
         <f>SUM(G$3:G14)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1056,7 +1121,7 @@
       </c>
       <c r="H15" s="8">
         <f>SUM(G$3:G15)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1068,7 +1133,7 @@
       </c>
       <c r="H16" s="8">
         <f>SUM(G$3:G16)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1080,7 +1145,7 @@
       </c>
       <c r="H17" s="8">
         <f>SUM(G$3:G17)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1092,7 +1157,7 @@
       </c>
       <c r="H18" s="8">
         <f>SUM(G$3:G18)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1104,7 +1169,7 @@
       </c>
       <c r="H19" s="8">
         <f>SUM(G$3:G19)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1116,7 +1181,7 @@
       </c>
       <c r="H20" s="8">
         <f>SUM(G$3:G20)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="21" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1128,7 +1193,7 @@
       </c>
       <c r="H21" s="8">
         <f>SUM(G$3:G21)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1140,7 +1205,7 @@
       </c>
       <c r="H22" s="8">
         <f>SUM(G$3:G22)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1152,7 +1217,7 @@
       </c>
       <c r="H23" s="8">
         <f>SUM(G$3:G23)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1164,7 +1229,7 @@
       </c>
       <c r="H24" s="8">
         <f>SUM(G$3:G24)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1175,7 +1240,7 @@
       </c>
       <c r="H25" s="8">
         <f>SUM(G$3:G25)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1186,7 +1251,7 @@
       </c>
       <c r="H26" s="8">
         <f>SUM(G$3:G26)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1197,7 +1262,7 @@
       </c>
       <c r="H27" s="8">
         <f>SUM(G$3:G27)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="28" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1208,7 +1273,7 @@
       </c>
       <c r="H28" s="8">
         <f>SUM(G$3:G28)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1219,7 +1284,7 @@
       </c>
       <c r="H29" s="8">
         <f>SUM(G$3:G29)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1230,7 +1295,7 @@
       </c>
       <c r="H30" s="8">
         <f>SUM(G$3:G30)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="31" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1241,7 +1306,7 @@
       </c>
       <c r="H31" s="8">
         <f>SUM(G$3:G31)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="32" spans="3:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1252,7 +1317,7 @@
       </c>
       <c r="H32" s="8">
         <f>SUM(G$3:G32)</f>
-        <v>0.28125000000000017</v>
+        <v>0.44097222222222254</v>
       </c>
     </row>
     <row r="33" spans="3:3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1327,7 +1392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9466DE97-788B-454A-A978-16D65412D85C}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>